<commit_message>
Added top emails in config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\proiect\Verificare_Facturi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B25E75F-4381-42BA-B7D3-5BB268E18D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A33B52-60E2-4226-99FA-1B46CC83A744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31230" yWindow="945" windowWidth="19095" windowHeight="16950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27765" yWindow="3525" windowWidth="30255" windowHeight="14805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Rezultat_VerificareFacturi_{0}.xlsx</t>
+  </si>
+  <si>
+    <t>topEmails</t>
+  </si>
+  <si>
+    <t>How many emails to be processed at a time(only use integer numbers)</t>
   </si>
 </sst>
 </file>
@@ -1776,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z54"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1980,214 +1986,225 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="75">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" ht="75">
+      <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>86</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>66</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>80</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>